<commit_message>
yema ny ghr p kiya
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AI-202505B1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\AI-202505B12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786BBCED-BF50-41DF-AB39-FA5CBFE99B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468BC295-8FD8-477D-9773-229544BDB703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{983E819B-A7BE-4369-BA8C-587A618C4069}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="2" xr2:uid="{983E819B-A7BE-4369-BA8C-587A618C4069}"/>
   </bookViews>
   <sheets>
     <sheet name="marksheet" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Id</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>hello</t>
+  </si>
+  <si>
+    <t>Hello This is kinza</t>
   </si>
 </sst>
 </file>
@@ -258,7 +261,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -283,21 +286,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1273,11 +1262,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5:M14">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
       <formula>80</formula>
       <formula>100</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>AND(ISNUMBER(I5),I5&gt;=0,I5&lt;=40)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1497,19 +1486,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K6">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="3">
+      <formula>LEN(TRIM(K6))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(K6))=0</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="3">
-      <formula>LEN(TRIM(K6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
-      <formula>LEN(TRIM(M6))=0</formula>
-    </cfRule>
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(M6))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="0" priority="2">
+      <formula>LEN(TRIM(M6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1523,17 +1512,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE0B74D-1F7A-4B7C-8BCA-96B038E2A4C9}">
-  <dimension ref="E7"/>
+  <dimension ref="E7:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>